<commit_message>
producers and leech expr
</commit_message>
<xml_diff>
--- a/Experiments/Part1-Uniform-MajorMinor/Part2-PeerPop.xlsx
+++ b/Experiments/Part1-Uniform-MajorMinor/Part2-PeerPop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,22 +33,22 @@
     <t>Taste 0 (PeerPop_Uniform)</t>
   </si>
   <si>
-    <t>Taste 1(PeerPop_MajorMinor)</t>
+    <t>Taste 1(PeerPop_Major)</t>
   </si>
   <si>
-    <t>Taste 0 (PeerPop-MajorMinor)</t>
+    <t>Taste 0 (PeerPop-Minor)</t>
   </si>
   <si>
-    <t>Taste 1 (PeerLikeSim_uniform)</t>
+    <t>Taste 1 (peer-follow-sim-uniform)</t>
   </si>
   <si>
-    <t>Taste 0 (PeerLikeSim_Unifrom)</t>
+    <t>Taste 0 (peer-follow-sim-uniform)</t>
   </si>
   <si>
-    <t>Taste 1(PeerLikeSim_MajorMinor)</t>
+    <t>Taste 0 (peer-follow-sim-Minor)</t>
   </si>
   <si>
-    <t>Taste 0 (PeerLikeSim_MajorMinor)</t>
+    <t>Taste 1 (peer-follow-sim-Major)</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1204,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Taste 1 (PeerLikeSim_uniform)</c:v>
+                  <c:v>Taste 1 (peer-follow-sim-uniform)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1219,154 +1219,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="85"/>
                 <c:pt idx="0">
-                  <c:v>2.386666666666663</c:v>
+                  <c:v>2.25333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.45333333333333</c:v>
+                  <c:v>5.826666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.17999999999997</c:v>
+                  <c:v>11.88666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.3733333333333</c:v>
+                  <c:v>19.1533333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.75333333333329</c:v>
+                  <c:v>26.57999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.17333333333329</c:v>
+                  <c:v>34.05333333333331</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.6533333333333</c:v>
+                  <c:v>41.55333333333331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51.1533333333333</c:v>
+                  <c:v>49.05333333333331</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58.6533333333333</c:v>
+                  <c:v>56.55333333333331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.15333333333329</c:v>
+                  <c:v>64.05333333333331</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>73.65333333333329</c:v>
+                  <c:v>71.55333333333331</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>81.15333333333329</c:v>
+                  <c:v>79.05333333333331</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>88.65333333333329</c:v>
+                  <c:v>86.55333333333331</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.15333333333329</c:v>
+                  <c:v>94.05333333333331</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>103.6533333333329</c:v>
+                  <c:v>101.5533333333331</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>111.1533333333329</c:v>
+                  <c:v>109.0533333333331</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>118.6466666666663</c:v>
+                  <c:v>116.5533333333331</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>126.0866666666663</c:v>
+                  <c:v>124.0533333333331</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>133.4266666666663</c:v>
+                  <c:v>131.5533333333331</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>140.6733333333331</c:v>
+                  <c:v>139.0199999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>147.8266666666663</c:v>
+                  <c:v>146.4599999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>154.8466666666663</c:v>
+                  <c:v>153.8399999999997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>161.6266666666663</c:v>
+                  <c:v>161.0533333333331</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>168.3866666666663</c:v>
+                  <c:v>168.113333333333</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>175.2333333333329</c:v>
+                  <c:v>175.0399999999996</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>181.8466666666664</c:v>
+                  <c:v>181.8733333333329</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>188.5466666666663</c:v>
+                  <c:v>188.453333333333</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>195.333333333333</c:v>
+                  <c:v>195.0999999999997</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>202.053333333333</c:v>
+                  <c:v>201.6733333333331</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>208.5866666666664</c:v>
+                  <c:v>208.313333333333</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>215.2066666666664</c:v>
+                  <c:v>214.7199999999997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>221.3599999999995</c:v>
+                  <c:v>220.7599999999997</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>227.8266666666664</c:v>
+                  <c:v>227.2333333333329</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>234.3066666666663</c:v>
+                  <c:v>233.4466666666663</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>240.3066666666664</c:v>
+                  <c:v>239.6333333333331</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>246.2599999999995</c:v>
+                  <c:v>245.9066666666662</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>251.7799999999997</c:v>
+                  <c:v>251.933333333333</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>256.8666666666662</c:v>
+                  <c:v>257.5533333333331</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>262.3999999999997</c:v>
+                  <c:v>263.053333333333</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>267.3599999999998</c:v>
+                  <c:v>267.353333333333</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>271.1599999999995</c:v>
+                  <c:v>271.873333333333</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>274.313333333333</c:v>
+                  <c:v>275.8066666666664</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>277.593333333333</c:v>
+                  <c:v>278.813333333333</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>280.1599999999997</c:v>
+                  <c:v>281.2599999999997</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>280.5599999999997</c:v>
+                  <c:v>282.7933333333331</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>280.6599999999996</c:v>
+                  <c:v>282.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>280.2133333333332</c:v>
+                  <c:v>281.4999999999999</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>278.6466666666664</c:v>
+                  <c:v>279.7266666666666</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>277.0466666666666</c:v>
+                  <c:v>277.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>274.9266666666666</c:v>
+                  <c:v>275.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>272.5</c:v>
@@ -1472,7 +1472,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Taste 0 (PeerLikeSim_Unifrom)</c:v>
+                  <c:v>Taste 0 (peer-follow-sim-uniform)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1487,154 +1487,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="85"/>
                 <c:pt idx="0">
-                  <c:v>2.606666666666663</c:v>
+                  <c:v>2.579999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.75333333333333</c:v>
+                  <c:v>6.279999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.53999999999997</c:v>
+                  <c:v>12.5733333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.84666666666662</c:v>
+                  <c:v>19.88666666666664</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.24666666666663</c:v>
+                  <c:v>27.32666666666664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.74666666666663</c:v>
+                  <c:v>34.82666666666664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44.17999999999996</c:v>
+                  <c:v>42.32666666666664</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51.67999999999997</c:v>
+                  <c:v>49.82666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>59.17999999999997</c:v>
+                  <c:v>57.32666666666664</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66.67999999999998</c:v>
+                  <c:v>64.82666666666664</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>74.17999999999998</c:v>
+                  <c:v>72.32666666666664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>81.67999999999998</c:v>
+                  <c:v>79.82666666666664</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>89.17999999999998</c:v>
+                  <c:v>87.32666666666664</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.67999999999998</c:v>
+                  <c:v>94.82666666666664</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>104.1799999999997</c:v>
+                  <c:v>102.3266666666664</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>111.6799999999997</c:v>
+                  <c:v>109.8266666666664</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>119.1799999999997</c:v>
+                  <c:v>117.3266666666664</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>126.6599999999997</c:v>
+                  <c:v>124.8266666666664</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>134.0533333333331</c:v>
+                  <c:v>132.3066666666664</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>141.3466666666664</c:v>
+                  <c:v>139.7066666666664</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>148.453333333333</c:v>
+                  <c:v>147.1599999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>155.2999999999996</c:v>
+                  <c:v>154.3733333333328</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>162.1266666666664</c:v>
+                  <c:v>161.4666666666664</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>168.893333333333</c:v>
+                  <c:v>168.3733333333331</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>175.7399999999997</c:v>
+                  <c:v>175.153333333333</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>182.6599999999997</c:v>
+                  <c:v>181.773333333333</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>189.6266666666663</c:v>
+                  <c:v>188.5999999999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>196.2399999999997</c:v>
+                  <c:v>195.3466666666663</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>202.6866666666663</c:v>
+                  <c:v>202.1199999999996</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>209.4266666666663</c:v>
+                  <c:v>208.5666666666665</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>215.793333333333</c:v>
+                  <c:v>214.7666666666663</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>221.9999999999995</c:v>
+                  <c:v>221.1466666666662</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>228.533333333333</c:v>
+                  <c:v>227.4999999999996</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>234.8999999999998</c:v>
+                  <c:v>233.6266666666663</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>240.6666666666664</c:v>
+                  <c:v>239.8066666666662</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>246.7199999999997</c:v>
+                  <c:v>245.5799999999996</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>252.4399999999995</c:v>
+                  <c:v>251.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>258.1933333333332</c:v>
+                  <c:v>257.1266666666664</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>263.753333333333</c:v>
+                  <c:v>262.6199999999996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>268.7066666666663</c:v>
+                  <c:v>267.693333333333</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>272.5866666666662</c:v>
+                  <c:v>271.6399999999997</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>276.4466666666662</c:v>
+                  <c:v>275.9333333333333</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>279.5333333333331</c:v>
+                  <c:v>279.273333333333</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>281.4266666666663</c:v>
+                  <c:v>281.1199999999998</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>282.0333333333332</c:v>
+                  <c:v>282.7133333333333</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>281.9799999999998</c:v>
+                  <c:v>282.7266666666664</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>281.1133333333332</c:v>
+                  <c:v>281.4999999999999</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>279.1999999999999</c:v>
+                  <c:v>279.66</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>277.1533333333333</c:v>
+                  <c:v>277.3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>274.9066666666666</c:v>
+                  <c:v>274.8133333333333</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>272.5</c:v>
@@ -1741,11 +1741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2121548296"/>
-        <c:axId val="2140895768"/>
+        <c:axId val="2146042328"/>
+        <c:axId val="2131966232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2121548296"/>
+        <c:axId val="2146042328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,7 +1773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140895768"/>
+        <c:crossAx val="2131966232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1781,7 +1781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140895768"/>
+        <c:axId val="2131966232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1811,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121548296"/>
+        <c:crossAx val="2146042328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2398,7 +2398,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Taste 1(PeerPop_MajorMinor)</c:v>
+                  <c:v>Taste 1(PeerPop_Major)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2666,7 +2666,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Taste 0 (PeerPop-MajorMinor)</c:v>
+                  <c:v>Taste 0 (PeerPop-Minor)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2934,7 +2934,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Taste 1(PeerLikeSim_MajorMinor)</c:v>
+                  <c:v>Taste 1 (peer-follow-sim-Major)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2952,145 +2952,145 @@
                   <c:v>2.44285714285714</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.190476190476186</c:v>
+                  <c:v>6.31428571428571</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.46666666666664</c:v>
+                  <c:v>13.07619047619042</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.91428571428568</c:v>
+                  <c:v>20.53333333333328</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.41428571428568</c:v>
+                  <c:v>28.02857142857136</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.90952380952378</c:v>
+                  <c:v>35.52857142857136</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.40952380952378</c:v>
+                  <c:v>43.02857142857137</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52.90952380952378</c:v>
+                  <c:v>50.52857142857137</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60.40952380952378</c:v>
+                  <c:v>58.02857142857137</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>67.9095238095238</c:v>
+                  <c:v>65.52857142857138</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>75.40952380952377</c:v>
+                  <c:v>73.02857142857138</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>82.90952380952377</c:v>
+                  <c:v>80.52857142857138</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90.4095238095238</c:v>
+                  <c:v>88.02857142857138</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>97.9095238095238</c:v>
+                  <c:v>95.52857142857138</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>105.4095238095233</c:v>
+                  <c:v>103.0285714285708</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>112.9095238095233</c:v>
+                  <c:v>110.5285714285708</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>120.4095238095233</c:v>
+                  <c:v>118.0285714285708</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>127.9095238095233</c:v>
+                  <c:v>125.5285714285708</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>135.4095238095233</c:v>
+                  <c:v>133.0285714285708</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>142.8952380952376</c:v>
+                  <c:v>140.5285714285708</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>150.2761904761899</c:v>
+                  <c:v>148.0285714285708</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>157.6285714285708</c:v>
+                  <c:v>155.5285714285708</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>164.9190476190471</c:v>
+                  <c:v>162.9904761904756</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>172.0047619047615</c:v>
+                  <c:v>170.4047619047613</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>178.8999999999997</c:v>
+                  <c:v>177.8476190476185</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>185.7904761904757</c:v>
+                  <c:v>184.77619047619</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>192.723809523809</c:v>
+                  <c:v>191.8523809523803</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>199.4666666666662</c:v>
+                  <c:v>198.8904761904757</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>206.0809523809518</c:v>
+                  <c:v>205.7761904761899</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>212.8095238095236</c:v>
+                  <c:v>212.5761904761901</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>219.6380952380947</c:v>
+                  <c:v>219.2904761904756</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>226.1095238095232</c:v>
+                  <c:v>225.9333333333327</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>232.5428571428566</c:v>
+                  <c:v>232.3619047619044</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>239.0952380952376</c:v>
+                  <c:v>238.9380952380947</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>245.4619047619042</c:v>
+                  <c:v>245.0666666666663</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>251.5952380952375</c:v>
+                  <c:v>251.2999999999995</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>257.6904761904757</c:v>
+                  <c:v>256.9952380952376</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>263.2857142857137</c:v>
+                  <c:v>262.9095238095232</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>268.2047619047615</c:v>
+                  <c:v>268.4619047619043</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>273.4238095238092</c:v>
+                  <c:v>273.519047619047</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>278.4904761904756</c:v>
+                  <c:v>278.1095238095232</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>282.3095238095234</c:v>
+                  <c:v>281.019047619047</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>285.6761904761901</c:v>
+                  <c:v>284.2285714285709</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>286.3952380952377</c:v>
+                  <c:v>285.2571428571425</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>285.5999999999998</c:v>
+                  <c:v>285.1285714285709</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>283.9285714285712</c:v>
+                  <c:v>284.0666666666665</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>281.795238095238</c:v>
+                  <c:v>282.2952380952379</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>279.9571428571428</c:v>
+                  <c:v>280.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>277.5</c:v>
@@ -3202,7 +3202,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Taste 0 (PeerLikeSim_MajorMinor)</c:v>
+                  <c:v>Taste 0 (peer-follow-sim-Minor)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3220,160 +3220,160 @@
                   <c:v>2.622222222222217</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.766666666666663</c:v>
+                  <c:v>5.266666666666661</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.66666666666662</c:v>
+                  <c:v>10.07777777777775</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.53333333333329</c:v>
+                  <c:v>16.76666666666662</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.78888888888886</c:v>
+                  <c:v>24.17777777777773</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.14444444444439</c:v>
+                  <c:v>31.67777777777773</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.4333333333333</c:v>
+                  <c:v>39.17777777777773</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48.77777777777773</c:v>
+                  <c:v>46.67777777777773</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56.2444444444444</c:v>
+                  <c:v>54.17777777777773</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63.7444444444444</c:v>
+                  <c:v>61.67777777777773</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71.2444444444444</c:v>
+                  <c:v>69.17777777777773</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>78.7444444444444</c:v>
+                  <c:v>76.67777777777772</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>86.2444444444444</c:v>
+                  <c:v>84.17777777777772</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>93.7444444444444</c:v>
+                  <c:v>91.67777777777772</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>101.1888888888886</c:v>
+                  <c:v>99.17777777777756</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>108.4555555555551</c:v>
+                  <c:v>106.6777777777773</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>115.5666666666661</c:v>
+                  <c:v>114.0666666666663</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>122.4333333333327</c:v>
+                  <c:v>121.4888888888885</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>129.0222222222218</c:v>
+                  <c:v>128.6666666666663</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>135.7111111111106</c:v>
+                  <c:v>135.7333333333328</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>142.244444444444</c:v>
+                  <c:v>142.644444444444</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>148.9888888888883</c:v>
+                  <c:v>149.2666666666662</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>155.344444444444</c:v>
+                  <c:v>155.8555555555551</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>161.944444444444</c:v>
+                  <c:v>162.0777777777774</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>168.2999999999996</c:v>
+                  <c:v>168.3555555555552</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>174.6222222222217</c:v>
+                  <c:v>174.7222222222218</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>180.7666666666661</c:v>
+                  <c:v>180.9111111111106</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>187.0111111111106</c:v>
+                  <c:v>187.3333333333329</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>193.544444444444</c:v>
+                  <c:v>193.5777777777774</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>199.7777777777775</c:v>
+                  <c:v>199.7222222222219</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>205.8555555555551</c:v>
+                  <c:v>206.0777777777774</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>211.5666666666663</c:v>
+                  <c:v>211.8111111111107</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>217.3555555555553</c:v>
+                  <c:v>217.5777777777775</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>223.3555555555551</c:v>
+                  <c:v>223.4777777777774</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>229.2777777777773</c:v>
+                  <c:v>229.2888888888884</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>233.9555555555551</c:v>
+                  <c:v>234.4333333333328</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>239.2444444444439</c:v>
+                  <c:v>240.3111111111106</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>244.644444444444</c:v>
+                  <c:v>245.4666666666663</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>248.9888888888884</c:v>
+                  <c:v>250.2666666666663</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>253.7222222222218</c:v>
+                  <c:v>255.033333333333</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>258.3999999999995</c:v>
+                  <c:v>259.2222222222218</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>262.1111111111107</c:v>
+                  <c:v>263.0999999999995</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>266.3888888888885</c:v>
+                  <c:v>266.6888888888885</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>269.366666666666</c:v>
+                  <c:v>269.1111111111106</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>271.1888888888885</c:v>
+                  <c:v>271.9888888888886</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>273.4666666666663</c:v>
+                  <c:v>273.5999999999996</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>274.322222222222</c:v>
+                  <c:v>274.4333333333329</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>274.6333333333329</c:v>
+                  <c:v>274.2666666666663</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>274.4111111111108</c:v>
+                  <c:v>274.1111111111109</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>272.9999999999998</c:v>
+                  <c:v>273.2999999999997</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>271.4333333333331</c:v>
+                  <c:v>271.3222222222221</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>269.4444444444444</c:v>
+                  <c:v>269.2888888888888</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>267.2111111111111</c:v>
+                  <c:v>267.1444444444444</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>264.8</c:v>
@@ -3382,19 +3382,19 @@
                   <c:v>262.3</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>259.8</c:v>
+                  <c:v>259.9111111111111</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>257.3</c:v>
+                  <c:v>257.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>254.8</c:v>
+                  <c:v>255.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>252.3</c:v>
+                  <c:v>252.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>249.8555555555555</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>247.5</c:v>
@@ -3471,11 +3471,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2105582440"/>
-        <c:axId val="-2105576824"/>
+        <c:axId val="2134254968"/>
+        <c:axId val="2134263448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2105582440"/>
+        <c:axId val="2134254968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3503,7 +3503,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105576824"/>
+        <c:crossAx val="2134263448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3511,7 +3511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105576824"/>
+        <c:axId val="2134263448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3546,7 +3546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105582440"/>
+        <c:crossAx val="2134254968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3957,8 +3957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O3" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3989,10 +3989,10 @@
         <v>7</v>
       </c>
       <c r="R1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" t="s">
         <v>8</v>
-      </c>
-      <c r="S1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="3:19">
@@ -4015,10 +4015,10 @@
         <v>1.3777777777777775</v>
       </c>
       <c r="N2">
-        <v>2.3866666666666627</v>
+        <v>2.2533333333333299</v>
       </c>
       <c r="O2">
-        <v>2.6066666666666629</v>
+        <v>2.579999999999997</v>
       </c>
       <c r="R2">
         <v>2.4428571428571391</v>
@@ -4047,16 +4047,16 @@
         <v>1.0888888888888828</v>
       </c>
       <c r="N3">
-        <v>7.4533333333333305</v>
+        <v>5.8266666666666636</v>
       </c>
       <c r="O3">
-        <v>7.7533333333333303</v>
+        <v>6.2799999999999949</v>
       </c>
       <c r="R3">
-        <v>8.1904761904761862</v>
+        <v>6.3142857142857096</v>
       </c>
       <c r="S3">
-        <v>6.7666666666666631</v>
+        <v>5.2666666666666613</v>
       </c>
     </row>
     <row r="4" spans="3:19">
@@ -4079,16 +4079,16 @@
         <v>-0.38888888888889472</v>
       </c>
       <c r="N4">
-        <v>14.17999999999997</v>
+        <v>11.886666666666631</v>
       </c>
       <c r="O4">
-        <v>14.539999999999969</v>
+        <v>12.573333333333299</v>
       </c>
       <c r="R4">
-        <v>15.466666666666637</v>
+        <v>13.076190476190419</v>
       </c>
       <c r="S4">
-        <v>12.666666666666623</v>
+        <v>10.077777777777753</v>
       </c>
     </row>
     <row r="5" spans="3:19">
@@ -4111,16 +4111,16 @@
         <v>-1.3444444444444428</v>
       </c>
       <c r="N5">
-        <v>21.373333333333299</v>
+        <v>19.1533333333333</v>
       </c>
       <c r="O5">
-        <v>21.846666666666621</v>
+        <v>19.886666666666638</v>
       </c>
       <c r="R5">
-        <v>22.914285714285679</v>
+        <v>20.533333333333278</v>
       </c>
       <c r="S5">
-        <v>19.533333333333292</v>
+        <v>16.766666666666623</v>
       </c>
     </row>
     <row r="6" spans="3:19">
@@ -4143,16 +4143,16 @@
         <v>-1.6555555555555366</v>
       </c>
       <c r="N6">
-        <v>28.753333333333295</v>
+        <v>26.579999999999977</v>
       </c>
       <c r="O6">
-        <v>29.246666666666631</v>
+        <v>27.326666666666643</v>
       </c>
       <c r="R6">
-        <v>30.414285714285683</v>
+        <v>28.028571428571365</v>
       </c>
       <c r="S6">
-        <v>26.788888888888856</v>
+        <v>24.177777777777731</v>
       </c>
     </row>
     <row r="7" spans="3:19">
@@ -4175,16 +4175,16 @@
         <v>-0.38888888888887624</v>
       </c>
       <c r="N7">
-        <v>36.173333333333289</v>
+        <v>34.053333333333313</v>
       </c>
       <c r="O7">
-        <v>36.746666666666627</v>
+        <v>34.82666666666664</v>
       </c>
       <c r="R7">
-        <v>37.909523809523783</v>
+        <v>35.528571428571368</v>
       </c>
       <c r="S7">
-        <v>34.144444444444389</v>
+        <v>31.677777777777731</v>
       </c>
     </row>
     <row r="8" spans="3:19">
@@ -4207,16 +4207,16 @@
         <v>1.4666666666666623</v>
       </c>
       <c r="N8">
-        <v>43.653333333333293</v>
+        <v>41.553333333333313</v>
       </c>
       <c r="O8">
-        <v>44.179999999999964</v>
+        <v>42.32666666666664</v>
       </c>
       <c r="R8">
-        <v>45.409523809523783</v>
+        <v>43.028571428571375</v>
       </c>
       <c r="S8">
-        <v>41.433333333333294</v>
+        <v>39.177777777777735</v>
       </c>
     </row>
     <row r="9" spans="3:19">
@@ -4239,16 +4239,16 @@
         <v>1.7222222222222112</v>
       </c>
       <c r="N9">
-        <v>51.153333333333293</v>
+        <v>49.053333333333313</v>
       </c>
       <c r="O9">
-        <v>51.679999999999971</v>
+        <v>49.82666666666664</v>
       </c>
       <c r="R9">
-        <v>52.909523809523783</v>
+        <v>50.528571428571375</v>
       </c>
       <c r="S9">
-        <v>48.777777777777729</v>
+        <v>46.677777777777735</v>
       </c>
     </row>
     <row r="10" spans="3:19">
@@ -4271,16 +4271,16 @@
         <v>2.9333333333333194</v>
       </c>
       <c r="N10">
-        <v>58.653333333333293</v>
+        <v>56.553333333333306</v>
       </c>
       <c r="O10">
-        <v>59.179999999999971</v>
+        <v>57.32666666666664</v>
       </c>
       <c r="R10">
-        <v>60.409523809523783</v>
+        <v>58.028571428571375</v>
       </c>
       <c r="S10">
-        <v>56.244444444444397</v>
+        <v>54.177777777777735</v>
       </c>
     </row>
     <row r="11" spans="3:19">
@@ -4303,16 +4303,16 @@
         <v>5.3888888888888697</v>
       </c>
       <c r="N11">
-        <v>66.153333333333293</v>
+        <v>64.053333333333313</v>
       </c>
       <c r="O11">
-        <v>66.679999999999978</v>
+        <v>64.82666666666664</v>
       </c>
       <c r="R11">
-        <v>67.90952380952379</v>
+        <v>65.528571428571382</v>
       </c>
       <c r="S11">
-        <v>63.744444444444397</v>
+        <v>61.677777777777735</v>
       </c>
     </row>
     <row r="12" spans="3:19">
@@ -4335,16 +4335,16 @@
         <v>6.9666666666666446</v>
       </c>
       <c r="N12">
-        <v>73.653333333333293</v>
+        <v>71.553333333333313</v>
       </c>
       <c r="O12">
-        <v>74.179999999999978</v>
+        <v>72.32666666666664</v>
       </c>
       <c r="R12">
-        <v>75.409523809523776</v>
+        <v>73.028571428571382</v>
       </c>
       <c r="S12">
-        <v>71.244444444444397</v>
+        <v>69.177777777777735</v>
       </c>
     </row>
     <row r="13" spans="3:19">
@@ -4367,16 +4367,16 @@
         <v>8.2999999999999652</v>
       </c>
       <c r="N13">
-        <v>81.153333333333293</v>
+        <v>79.053333333333313</v>
       </c>
       <c r="O13">
-        <v>81.679999999999978</v>
+        <v>79.82666666666664</v>
       </c>
       <c r="R13">
-        <v>82.909523809523776</v>
+        <v>80.528571428571382</v>
       </c>
       <c r="S13">
-        <v>78.744444444444397</v>
+        <v>76.67777777777772</v>
       </c>
     </row>
     <row r="14" spans="3:19">
@@ -4399,16 +4399,16 @@
         <v>8.3666666666666458</v>
       </c>
       <c r="N14">
-        <v>88.653333333333293</v>
+        <v>86.553333333333313</v>
       </c>
       <c r="O14">
-        <v>89.179999999999978</v>
+        <v>87.32666666666664</v>
       </c>
       <c r="R14">
-        <v>90.40952380952379</v>
+        <v>88.028571428571382</v>
       </c>
       <c r="S14">
-        <v>86.244444444444412</v>
+        <v>84.17777777777772</v>
       </c>
     </row>
     <row r="15" spans="3:19">
@@ -4431,16 +4431,16 @@
         <v>9.9222222222222136</v>
       </c>
       <c r="N15">
-        <v>96.153333333333293</v>
+        <v>94.053333333333313</v>
       </c>
       <c r="O15">
-        <v>96.679999999999978</v>
+        <v>94.82666666666664</v>
       </c>
       <c r="R15">
-        <v>97.90952380952379</v>
+        <v>95.528571428571382</v>
       </c>
       <c r="S15">
-        <v>93.744444444444412</v>
+        <v>91.67777777777772</v>
       </c>
     </row>
     <row r="16" spans="3:19">
@@ -4463,16 +4463,16 @@
         <v>12.111111111111088</v>
       </c>
       <c r="N16">
-        <v>103.65333333333292</v>
+        <v>101.55333333333309</v>
       </c>
       <c r="O16">
-        <v>104.17999999999972</v>
+        <v>102.3266666666664</v>
       </c>
       <c r="R16">
-        <v>105.40952380952331</v>
+        <v>103.02857142857079</v>
       </c>
       <c r="S16">
-        <v>101.1888888888886</v>
+        <v>99.177777777777564</v>
       </c>
     </row>
     <row r="17" spans="3:19">
@@ -4495,16 +4495,16 @@
         <v>11.622222222222199</v>
       </c>
       <c r="N17">
-        <v>111.15333333333292</v>
+        <v>109.0533333333331</v>
       </c>
       <c r="O17">
-        <v>111.67999999999972</v>
+        <v>109.8266666666664</v>
       </c>
       <c r="R17">
-        <v>112.90952380952331</v>
+        <v>110.52857142857079</v>
       </c>
       <c r="S17">
-        <v>108.45555555555509</v>
+        <v>106.67777777777731</v>
       </c>
     </row>
     <row r="18" spans="3:19">
@@ -4527,16 +4527,16 @@
         <v>11.766666666666643</v>
       </c>
       <c r="N18">
-        <v>118.64666666666631</v>
+        <v>116.5533333333331</v>
       </c>
       <c r="O18">
-        <v>119.17999999999972</v>
+        <v>117.3266666666664</v>
       </c>
       <c r="R18">
-        <v>120.40952380952331</v>
+        <v>118.02857142857079</v>
       </c>
       <c r="S18">
-        <v>115.56666666666608</v>
+        <v>114.06666666666629</v>
       </c>
     </row>
     <row r="19" spans="3:19">
@@ -4559,16 +4559,16 @@
         <v>15.455555555555502</v>
       </c>
       <c r="N19">
-        <v>126.08666666666632</v>
+        <v>124.0533333333331</v>
       </c>
       <c r="O19">
-        <v>126.65999999999971</v>
+        <v>124.8266666666664</v>
       </c>
       <c r="R19">
-        <v>127.90952380952331</v>
+        <v>125.52857142857079</v>
       </c>
       <c r="S19">
-        <v>122.43333333333271</v>
+        <v>121.48888888888851</v>
       </c>
     </row>
     <row r="20" spans="3:19">
@@ -4591,16 +4591,16 @@
         <v>17.077777777777733</v>
       </c>
       <c r="N20">
-        <v>133.42666666666634</v>
+        <v>131.55333333333311</v>
       </c>
       <c r="O20">
-        <v>134.05333333333311</v>
+        <v>132.30666666666639</v>
       </c>
       <c r="R20">
-        <v>135.40952380952334</v>
+        <v>133.02857142857079</v>
       </c>
       <c r="S20">
-        <v>129.02222222222181</v>
+        <v>128.66666666666629</v>
       </c>
     </row>
     <row r="21" spans="3:19">
@@ -4623,16 +4623,16 @@
         <v>18.311111111111053</v>
       </c>
       <c r="N21">
-        <v>140.67333333333312</v>
+        <v>139.0199999999997</v>
       </c>
       <c r="O21">
-        <v>141.34666666666641</v>
+        <v>139.70666666666639</v>
       </c>
       <c r="R21">
-        <v>142.89523809523763</v>
+        <v>140.52857142857079</v>
       </c>
       <c r="S21">
-        <v>135.7111111111106</v>
+        <v>135.73333333333281</v>
       </c>
     </row>
     <row r="22" spans="3:19">
@@ -4655,16 +4655,16 @@
         <v>21.255555555555496</v>
       </c>
       <c r="N22">
-        <v>147.82666666666628</v>
+        <v>146.45999999999972</v>
       </c>
       <c r="O22">
-        <v>148.45333333333303</v>
+        <v>147.1599999999998</v>
       </c>
       <c r="R22">
-        <v>150.27619047618992</v>
+        <v>148.02857142857079</v>
       </c>
       <c r="S22">
-        <v>142.24444444444401</v>
+        <v>142.64444444444399</v>
       </c>
     </row>
     <row r="23" spans="3:19">
@@ -4687,16 +4687,16 @@
         <v>22.25555555555551</v>
       </c>
       <c r="N23">
-        <v>154.84666666666629</v>
+        <v>153.83999999999969</v>
       </c>
       <c r="O23">
-        <v>155.29999999999959</v>
+        <v>154.37333333333282</v>
       </c>
       <c r="R23">
-        <v>157.62857142857081</v>
+        <v>155.52857142857079</v>
       </c>
       <c r="S23">
-        <v>148.98888888888831</v>
+        <v>149.2666666666662</v>
       </c>
     </row>
     <row r="24" spans="3:19">
@@ -4719,16 +4719,16 @@
         <v>22.666666666666611</v>
       </c>
       <c r="N24">
-        <v>161.62666666666627</v>
+        <v>161.05333333333311</v>
       </c>
       <c r="O24">
-        <v>162.12666666666638</v>
+        <v>161.46666666666641</v>
       </c>
       <c r="R24">
-        <v>164.91904761904709</v>
+        <v>162.99047619047559</v>
       </c>
       <c r="S24">
-        <v>155.34444444444404</v>
+        <v>155.8555555555551</v>
       </c>
     </row>
     <row r="25" spans="3:19">
@@ -4751,16 +4751,16 @@
         <v>25.288888888888845</v>
       </c>
       <c r="N25">
-        <v>168.38666666666629</v>
+        <v>168.113333333333</v>
       </c>
       <c r="O25">
-        <v>168.89333333333298</v>
+        <v>168.37333333333314</v>
       </c>
       <c r="R25">
-        <v>172.00476190476147</v>
+        <v>170.4047619047613</v>
       </c>
       <c r="S25">
-        <v>161.94444444444403</v>
+        <v>162.07777777777738</v>
       </c>
     </row>
     <row r="26" spans="3:19">
@@ -4783,16 +4783,16 @@
         <v>26.666666666666622</v>
       </c>
       <c r="N26">
-        <v>175.23333333333289</v>
+        <v>175.03999999999962</v>
       </c>
       <c r="O26">
-        <v>175.73999999999972</v>
+        <v>175.15333333333291</v>
       </c>
       <c r="R26">
-        <v>178.89999999999969</v>
+        <v>177.84761904761848</v>
       </c>
       <c r="S26">
-        <v>168.29999999999956</v>
+        <v>168.35555555555518</v>
       </c>
     </row>
     <row r="27" spans="3:19">
@@ -4815,16 +4815,16 @@
         <v>28.755555555555521</v>
       </c>
       <c r="N27">
-        <v>181.84666666666641</v>
+        <v>181.87333333333288</v>
       </c>
       <c r="O27">
-        <v>182.65999999999968</v>
+        <v>181.77333333333303</v>
       </c>
       <c r="R27">
-        <v>185.79047619047569</v>
+        <v>184.77619047619004</v>
       </c>
       <c r="S27">
-        <v>174.62222222222172</v>
+        <v>174.72222222222177</v>
       </c>
     </row>
     <row r="28" spans="3:19">
@@ -4847,16 +4847,16 @@
         <v>30.855555555555508</v>
       </c>
       <c r="N28">
-        <v>188.54666666666628</v>
+        <v>188.45333333333298</v>
       </c>
       <c r="O28">
-        <v>189.62666666666632</v>
+        <v>188.59999999999971</v>
       </c>
       <c r="R28">
-        <v>192.723809523809</v>
+        <v>191.85238095238037</v>
       </c>
       <c r="S28">
-        <v>180.76666666666611</v>
+        <v>180.91111111111061</v>
       </c>
     </row>
     <row r="29" spans="3:19">
@@ -4879,16 +4879,16 @@
         <v>33.144444444444396</v>
       </c>
       <c r="N29">
-        <v>195.333333333333</v>
+        <v>195.09999999999971</v>
       </c>
       <c r="O29">
-        <v>196.23999999999972</v>
+        <v>195.34666666666629</v>
       </c>
       <c r="R29">
-        <v>199.46666666666621</v>
+        <v>198.89047619047571</v>
       </c>
       <c r="S29">
-        <v>187.01111111111061</v>
+        <v>187.33333333333289</v>
       </c>
     </row>
     <row r="30" spans="3:19">
@@ -4911,16 +4911,16 @@
         <v>34.288888888888849</v>
       </c>
       <c r="N30">
-        <v>202.053333333333</v>
+        <v>201.67333333333309</v>
       </c>
       <c r="O30">
-        <v>202.68666666666627</v>
+        <v>202.11999999999961</v>
       </c>
       <c r="R30">
-        <v>206.0809523809518</v>
+        <v>205.77619047618992</v>
       </c>
       <c r="S30">
-        <v>193.54444444444397</v>
+        <v>193.57777777777738</v>
       </c>
     </row>
     <row r="31" spans="3:19">
@@ -4943,16 +4943,16 @@
         <v>35.333333333333272</v>
       </c>
       <c r="N31">
-        <v>208.58666666666642</v>
+        <v>208.31333333333299</v>
       </c>
       <c r="O31">
-        <v>209.42666666666628</v>
+        <v>208.56666666666652</v>
       </c>
       <c r="R31">
-        <v>212.80952380952363</v>
+        <v>212.57619047619011</v>
       </c>
       <c r="S31">
-        <v>199.77777777777752</v>
+        <v>199.72222222222189</v>
       </c>
     </row>
     <row r="32" spans="3:19">
@@ -4975,16 +4975,16 @@
         <v>36.533333333333282</v>
       </c>
       <c r="N32">
-        <v>215.20666666666639</v>
+        <v>214.71999999999966</v>
       </c>
       <c r="O32">
-        <v>215.79333333333301</v>
+        <v>214.76666666666628</v>
       </c>
       <c r="R32">
-        <v>219.63809523809468</v>
+        <v>219.2904761904756</v>
       </c>
       <c r="S32">
-        <v>205.8555555555551</v>
+        <v>206.07777777777741</v>
       </c>
     </row>
     <row r="33" spans="3:19">
@@ -5007,16 +5007,16 @@
         <v>39.122222222222206</v>
       </c>
       <c r="N33">
-        <v>221.3599999999995</v>
+        <v>220.75999999999971</v>
       </c>
       <c r="O33">
-        <v>221.99999999999949</v>
+        <v>221.14666666666625</v>
       </c>
       <c r="R33">
-        <v>226.10952380952321</v>
+        <v>225.93333333333266</v>
       </c>
       <c r="S33">
-        <v>211.56666666666629</v>
+        <v>211.81111111111073</v>
       </c>
     </row>
     <row r="34" spans="3:19">
@@ -5039,16 +5039,16 @@
         <v>41.133333333333283</v>
       </c>
       <c r="N34">
-        <v>227.82666666666643</v>
+        <v>227.23333333333289</v>
       </c>
       <c r="O34">
-        <v>228.53333333333302</v>
+        <v>227.4999999999996</v>
       </c>
       <c r="R34">
-        <v>232.5428571428566</v>
+        <v>232.36190476190441</v>
       </c>
       <c r="S34">
-        <v>217.3555555555553</v>
+        <v>217.5777777777775</v>
       </c>
     </row>
     <row r="35" spans="3:19">
@@ -5071,16 +5071,16 @@
         <v>42.799999999999969</v>
       </c>
       <c r="N35">
-        <v>234.30666666666633</v>
+        <v>233.44666666666632</v>
       </c>
       <c r="O35">
-        <v>234.89999999999981</v>
+        <v>233.62666666666632</v>
       </c>
       <c r="R35">
-        <v>239.09523809523756</v>
+        <v>238.93809523809469</v>
       </c>
       <c r="S35">
-        <v>223.3555555555551</v>
+        <v>223.47777777777742</v>
       </c>
     </row>
     <row r="36" spans="3:19">
@@ -5103,16 +5103,16 @@
         <v>45.044444444444402</v>
       </c>
       <c r="N36">
-        <v>240.30666666666639</v>
+        <v>239.63333333333307</v>
       </c>
       <c r="O36">
-        <v>240.66666666666637</v>
+        <v>239.80666666666622</v>
       </c>
       <c r="R36">
-        <v>245.46190476190424</v>
+        <v>245.06666666666629</v>
       </c>
       <c r="S36">
-        <v>229.27777777777732</v>
+        <v>229.28888888888838</v>
       </c>
     </row>
     <row r="37" spans="3:19">
@@ -5135,16 +5135,16 @@
         <v>47.555555555555515</v>
       </c>
       <c r="N37">
-        <v>246.25999999999948</v>
+        <v>245.90666666666621</v>
       </c>
       <c r="O37">
-        <v>246.71999999999971</v>
+        <v>245.57999999999964</v>
       </c>
       <c r="R37">
-        <v>251.59523809523753</v>
+        <v>251.2999999999995</v>
       </c>
       <c r="S37">
-        <v>233.95555555555507</v>
+        <v>234.4333333333328</v>
       </c>
     </row>
     <row r="38" spans="3:19">
@@ -5167,16 +5167,16 @@
         <v>50.111111111111065</v>
       </c>
       <c r="N38">
-        <v>251.77999999999975</v>
+        <v>251.933333333333</v>
       </c>
       <c r="O38">
-        <v>252.43999999999951</v>
+        <v>251.39999999999958</v>
       </c>
       <c r="R38">
-        <v>257.69047619047569</v>
+        <v>256.9952380952376</v>
       </c>
       <c r="S38">
-        <v>239.2444444444439</v>
+        <v>240.31111111111059</v>
       </c>
     </row>
     <row r="39" spans="3:19">
@@ -5199,16 +5199,16 @@
         <v>52.422222222222182</v>
       </c>
       <c r="N39">
-        <v>256.86666666666622</v>
+        <v>257.55333333333311</v>
       </c>
       <c r="O39">
-        <v>258.19333333333327</v>
+        <v>257.12666666666638</v>
       </c>
       <c r="R39">
-        <v>263.28571428571365</v>
+        <v>262.90952380952319</v>
       </c>
       <c r="S39">
-        <v>244.64444444444402</v>
+        <v>245.46666666666633</v>
       </c>
     </row>
     <row r="40" spans="3:19">
@@ -5231,16 +5231,16 @@
         <v>54.633333333333283</v>
       </c>
       <c r="N40">
-        <v>262.39999999999969</v>
+        <v>263.05333333333294</v>
       </c>
       <c r="O40">
-        <v>263.75333333333299</v>
+        <v>262.61999999999961</v>
       </c>
       <c r="R40">
-        <v>268.2047619047616</v>
+        <v>268.46190476190429</v>
       </c>
       <c r="S40">
-        <v>248.98888888888843</v>
+        <v>250.26666666666628</v>
       </c>
     </row>
     <row r="41" spans="3:19">
@@ -5263,16 +5263,16 @@
         <v>56.099999999999945</v>
       </c>
       <c r="N41">
-        <v>267.35999999999984</v>
+        <v>267.35333333333301</v>
       </c>
       <c r="O41">
-        <v>268.70666666666631</v>
+        <v>267.69333333333304</v>
       </c>
       <c r="R41">
-        <v>273.42380952380915</v>
+        <v>273.51904761904706</v>
       </c>
       <c r="S41">
-        <v>253.7222222222218</v>
+        <v>255.03333333333302</v>
       </c>
     </row>
     <row r="42" spans="3:19">
@@ -5295,16 +5295,16 @@
         <v>59.211111111111066</v>
       </c>
       <c r="N42">
-        <v>271.15999999999951</v>
+        <v>271.87333333333299</v>
       </c>
       <c r="O42">
-        <v>272.58666666666619</v>
+        <v>271.6399999999997</v>
       </c>
       <c r="R42">
-        <v>278.49047619047559</v>
+        <v>278.10952380952324</v>
       </c>
       <c r="S42">
-        <v>258.39999999999952</v>
+        <v>259.22222222222183</v>
       </c>
     </row>
     <row r="43" spans="3:19">
@@ -5327,16 +5327,16 @@
         <v>61.13333333333329</v>
       </c>
       <c r="N43">
-        <v>274.31333333333305</v>
+        <v>275.80666666666639</v>
       </c>
       <c r="O43">
-        <v>276.44666666666626</v>
+        <v>275.93333333333328</v>
       </c>
       <c r="R43">
-        <v>282.30952380952345</v>
+        <v>281.01904761904706</v>
       </c>
       <c r="S43">
-        <v>262.11111111111069</v>
+        <v>263.09999999999951</v>
       </c>
     </row>
     <row r="44" spans="3:19">
@@ -5359,16 +5359,16 @@
         <v>62.97777777777776</v>
       </c>
       <c r="N44">
-        <v>277.59333333333302</v>
+        <v>278.81333333333299</v>
       </c>
       <c r="O44">
-        <v>279.53333333333308</v>
+        <v>279.27333333333291</v>
       </c>
       <c r="R44">
-        <v>285.67619047619007</v>
+        <v>284.22857142857089</v>
       </c>
       <c r="S44">
-        <v>266.38888888888852</v>
+        <v>266.68888888888853</v>
       </c>
     </row>
     <row r="45" spans="3:19">
@@ -5391,16 +5391,16 @@
         <v>64.499999999999957</v>
       </c>
       <c r="N45">
-        <v>280.15999999999968</v>
+        <v>281.25999999999971</v>
       </c>
       <c r="O45">
-        <v>281.42666666666634</v>
+        <v>281.11999999999978</v>
       </c>
       <c r="R45">
-        <v>286.39523809523769</v>
+        <v>285.25714285714247</v>
       </c>
       <c r="S45">
-        <v>269.36666666666605</v>
+        <v>269.11111111111057</v>
       </c>
     </row>
     <row r="46" spans="3:19">
@@ -5423,16 +5423,16 @@
         <v>67.922222222222189</v>
       </c>
       <c r="N46">
-        <v>280.55999999999966</v>
+        <v>282.79333333333312</v>
       </c>
       <c r="O46">
-        <v>282.03333333333319</v>
+        <v>282.71333333333331</v>
       </c>
       <c r="R46">
-        <v>285.5999999999998</v>
+        <v>285.12857142857092</v>
       </c>
       <c r="S46">
-        <v>271.18888888888847</v>
+        <v>271.9888888888886</v>
       </c>
     </row>
     <row r="47" spans="3:19">
@@ -5455,16 +5455,16 @@
         <v>69.966666666666626</v>
       </c>
       <c r="N47">
-        <v>280.65999999999957</v>
+        <v>282.69999999999982</v>
       </c>
       <c r="O47">
-        <v>281.97999999999979</v>
+        <v>282.7266666666664</v>
       </c>
       <c r="R47">
-        <v>283.92857142857122</v>
+        <v>284.06666666666649</v>
       </c>
       <c r="S47">
-        <v>273.4666666666663</v>
+        <v>273.59999999999957</v>
       </c>
     </row>
     <row r="48" spans="3:19">
@@ -5487,16 +5487,16 @@
         <v>70.988888888888852</v>
       </c>
       <c r="N48">
-        <v>280.2133333333332</v>
+        <v>281.49999999999989</v>
       </c>
       <c r="O48">
-        <v>281.11333333333323</v>
+        <v>281.49999999999989</v>
       </c>
       <c r="R48">
-        <v>281.79523809523801</v>
+        <v>282.29523809523789</v>
       </c>
       <c r="S48">
-        <v>274.32222222222191</v>
+        <v>274.43333333333288</v>
       </c>
     </row>
     <row r="49" spans="3:19">
@@ -5519,16 +5519,16 @@
         <v>74.399999999999963</v>
       </c>
       <c r="N49">
-        <v>278.64666666666648</v>
+        <v>279.72666666666657</v>
       </c>
       <c r="O49">
-        <v>279.19999999999993</v>
+        <v>279.65999999999991</v>
       </c>
       <c r="R49">
-        <v>279.9571428571428</v>
+        <v>280</v>
       </c>
       <c r="S49">
-        <v>274.63333333333287</v>
+        <v>274.26666666666631</v>
       </c>
     </row>
     <row r="50" spans="3:19">
@@ -5551,16 +5551,16 @@
         <v>77.233333333333277</v>
       </c>
       <c r="N50">
-        <v>277.04666666666662</v>
+        <v>277.5</v>
       </c>
       <c r="O50">
-        <v>277.15333333333331</v>
+        <v>277.3</v>
       </c>
       <c r="R50">
         <v>277.5</v>
       </c>
       <c r="S50">
-        <v>274.41111111111076</v>
+        <v>274.11111111111092</v>
       </c>
     </row>
     <row r="51" spans="3:19">
@@ -5583,16 +5583,16 @@
         <v>81.1666666666666</v>
       </c>
       <c r="N51">
-        <v>274.92666666666662</v>
+        <v>275</v>
       </c>
       <c r="O51">
-        <v>274.90666666666658</v>
+        <v>274.81333333333333</v>
       </c>
       <c r="R51">
         <v>275</v>
       </c>
       <c r="S51">
-        <v>272.99999999999977</v>
+        <v>273.29999999999967</v>
       </c>
     </row>
     <row r="52" spans="3:19">
@@ -5624,7 +5624,7 @@
         <v>272.5</v>
       </c>
       <c r="S52">
-        <v>271.43333333333305</v>
+        <v>271.32222222222208</v>
       </c>
     </row>
     <row r="53" spans="3:19">
@@ -5656,7 +5656,7 @@
         <v>270</v>
       </c>
       <c r="S53">
-        <v>269.4444444444444</v>
+        <v>269.28888888888878</v>
       </c>
     </row>
     <row r="54" spans="3:19">
@@ -5688,7 +5688,7 @@
         <v>267.5</v>
       </c>
       <c r="S54">
-        <v>267.21111111111111</v>
+        <v>267.14444444444439</v>
       </c>
     </row>
     <row r="55" spans="3:19">
@@ -5784,7 +5784,7 @@
         <v>260</v>
       </c>
       <c r="S57">
-        <v>259.8</v>
+        <v>259.9111111111111</v>
       </c>
     </row>
     <row r="58" spans="3:19">
@@ -5816,7 +5816,7 @@
         <v>257.5</v>
       </c>
       <c r="S58">
-        <v>257.3</v>
+        <v>257.5</v>
       </c>
     </row>
     <row r="59" spans="3:19">
@@ -5848,7 +5848,7 @@
         <v>255</v>
       </c>
       <c r="S59">
-        <v>254.8</v>
+        <v>255</v>
       </c>
     </row>
     <row r="60" spans="3:19">
@@ -5880,7 +5880,7 @@
         <v>252.5</v>
       </c>
       <c r="S60">
-        <v>252.3</v>
+        <v>252.5</v>
       </c>
     </row>
     <row r="61" spans="3:19">
@@ -5912,7 +5912,7 @@
         <v>250</v>
       </c>
       <c r="S61">
-        <v>249.85555555555547</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="3:19">

</xml_diff>